<commit_message>
Folosim webdriverwait, speednormal este varianta normala si optimized prima optimizare
</commit_message>
<xml_diff>
--- a/seap_results.xlsx
+++ b/seap_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeapMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D3BBA8-1816-4CEA-BEE5-E0731C6EDD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5CB974-4C5E-420D-A7A8-F9A604AA7787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="178">
   <si>
     <t>Data detectării</t>
   </si>
@@ -397,6 +397,9 @@
     <t>04.06.2025 11:00</t>
   </si>
   <si>
+    <t>Lipsa Stoc</t>
+  </si>
+  <si>
     <t>ADV1484308</t>
   </si>
   <si>
@@ -439,7 +442,118 @@
     <t>06.06.2025 10:30</t>
   </si>
   <si>
-    <t>Lipsa Stoc</t>
+    <t>2025-05-30 14:09:47</t>
+  </si>
+  <si>
+    <t>ADV1484429</t>
+  </si>
+  <si>
+    <t>Execuție fundații la stâlpii din cadrul celor 3 lucrări de investiții „M-21-T006 Lucrare de intarire retea in amonte de punctul de racordare-realizare racord 20kV si post de transformare Chiuzabaia Groape” „M-23-T101 Intarire retea in amonte de punctul de racordare - realizare circuit 0,4 kV din PT</t>
+  </si>
+  <si>
+    <t>05.06.2025 14:00</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:09:53</t>
+  </si>
+  <si>
+    <t>ADV1484401</t>
+  </si>
+  <si>
+    <t>Scule de mana si materile electrice</t>
+  </si>
+  <si>
+    <t>02.06.2025 16:00</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:10:17</t>
+  </si>
+  <si>
+    <t>ADV1484402</t>
+  </si>
+  <si>
+    <t>Achizitie cabluri date</t>
+  </si>
+  <si>
+    <t>03.06.2025 13:39</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:10:45</t>
+  </si>
+  <si>
+    <t>ADV1484409</t>
+  </si>
+  <si>
+    <t>Lampa led iluminat stradal</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:10:53</t>
+  </si>
+  <si>
+    <t>ADV1484420</t>
+  </si>
+  <si>
+    <t>stabilizator de tensiune pt. echipament de tomografie Siemens Somatom Scope Power</t>
+  </si>
+  <si>
+    <t>stabilizator</t>
+  </si>
+  <si>
+    <t>02.06.2025 12:00</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:11:18</t>
+  </si>
+  <si>
+    <t>ADV1484361</t>
+  </si>
+  <si>
+    <t>Realizare releveu arhitectural si topografic</t>
+  </si>
+  <si>
+    <t>rele</t>
+  </si>
+  <si>
+    <t>06.06.2025 23:30</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:14:45</t>
+  </si>
+  <si>
+    <t>ADV1484443</t>
+  </si>
+  <si>
+    <t>COȘERIT - CURĂȚARE COȘ DE FUM</t>
+  </si>
+  <si>
+    <t>sigurante</t>
+  </si>
+  <si>
+    <t>04.06.2025 08:00</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:15:19</t>
+  </si>
+  <si>
+    <t>ADV1484444</t>
+  </si>
+  <si>
+    <t>Materiale electrice</t>
+  </si>
+  <si>
+    <t>echipamente de laborator</t>
+  </si>
+  <si>
+    <t>03.06.2025 10:00</t>
+  </si>
+  <si>
+    <t>2025-05-30 14:17:31</t>
+  </si>
+  <si>
+    <t>ADV1484445</t>
+  </si>
+  <si>
+    <t>Agent Frigorific- Freon</t>
   </si>
 </sst>
 </file>
@@ -786,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1265,6 +1379,9 @@
       <c r="E25" t="s">
         <v>49</v>
       </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1383,7 +1500,7 @@
         <v>124</v>
       </c>
       <c r="F31" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1391,16 +1508,16 @@
         <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s">
         <v>123</v>
       </c>
       <c r="E32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F32" t="s">
         <v>88</v>
@@ -1408,19 +1525,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D33" t="s">
         <v>62</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
         <v>88</v>
@@ -1428,19 +1545,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s">
         <v>21</v>
       </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F34" t="s">
         <v>88</v>
@@ -1448,21 +1565,195 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
         <v>21</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" t="s">
+        <v>164</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" t="s">
+        <v>168</v>
+      </c>
+      <c r="E42" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>